<commit_message>
Creacion de documento Maestro de muestreo de datos, arreglo de muestreos en centro de evento y pagos, y arreglo de diagramas
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/CentroEventos - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/CentroEventos - Muestreo Datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\ModeloDominio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO/SpaOnline/ModeloDominio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AD09FB-8689-4518-ADAE-2F2E39831A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{35AD09FB-8689-4518-ADAE-2F2E39831A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBF0DF63-1C05-4C82-BAFE-70BD0D31E1B0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="774" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -84,15 +84,6 @@
     <t>Combinacion única</t>
   </si>
   <si>
-    <t>Transacción 1</t>
-  </si>
-  <si>
-    <t>Transacción 2</t>
-  </si>
-  <si>
-    <t>Transacción N</t>
-  </si>
-  <si>
     <t>Eventos</t>
   </si>
   <si>
@@ -100,6 +91,21 @@
   </si>
   <si>
     <t>Objeto de dominio que contiene la informacion de los eventos que realiza el Spa</t>
+  </si>
+  <si>
+    <t>OfertaFacial</t>
+  </si>
+  <si>
+    <t>Notificado</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Reserva - 1</t>
+  </si>
+  <si>
+    <t>Factura 1</t>
   </si>
 </sst>
 </file>
@@ -210,17 +216,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>267056</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>181266</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>124347</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C93D77A-7774-6DD1-DEAC-25110BC320A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45B88307-E103-D674-45AE-E032BF61272F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -237,7 +243,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2553056" cy="2086266"/>
+          <a:ext cx="5372850" cy="3743847"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -630,16 +636,16 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -650,64 +656,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="str">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="str">
         <f>B2</f>
-        <v>Transacción 1</v>
+        <v>OfertaFacial</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C4" si="0">B3</f>
-        <v>Transacción 2</v>
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f t="shared" ref="D3:D4" si="0">B3</f>
+        <v>Reserva - 1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="str">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Transacción N</v>
+        <v>Factura 1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>